<commit_message>
Se agrega columna con el tipo de renta
Esta puede ser FIJA o VARIABLE, y depende de si se informa la fecha en el documento o no. Además se corrige el process_date a utilizar en el main call.
</commit_message>
<xml_diff>
--- a/Nevasa/Renta/20240821/20240821_nevasa_renta_results.xlsx
+++ b/Nevasa/Renta/20240821/20240821_nevasa_renta_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,35 +440,40 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>tipo_renta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>liquidacion</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>fecha_pago</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>documento</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>precio</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>cantidad</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>compra</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>venta</t>
         </is>
@@ -477,54 +482,64 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>FIJA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>PM</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="C2" s="2" t="n">
         <v>45525</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>BCHIDU0716</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>96.504</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>200000000</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>194171674</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>VARIABLE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>PH</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="C3" s="2" t="n">
         <v>45524</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>CFINHRFLA</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>16378.93</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>611</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>10007526</v>
       </c>
     </row>

</xml_diff>